<commit_message>
commit from ahmed 13 June
</commit_message>
<xml_diff>
--- a/code explanation/FIles explanations.xlsx
+++ b/code explanation/FIles explanations.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5019B29F-8501-487A-9AF4-2FCAA18B285B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D8AEE8-C429-4725-A5E2-F4EE50736EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="126">
   <si>
     <t>MdiADoFunctions</t>
   </si>
@@ -404,6 +404,9 @@
   </si>
   <si>
     <t>Create</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -426,7 +429,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -436,6 +439,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -452,12 +467,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -891,14 +908,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="43.21875" customWidth="1"/>
     <col min="2" max="2" width="46.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -919,6 +937,9 @@
       <c r="B2" t="s">
         <v>32</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -927,6 +948,9 @@
       <c r="B3" t="s">
         <v>10</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -935,8 +959,8 @@
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -946,16 +970,16 @@
       <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -964,8 +988,8 @@
       <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
-        <v>12</v>
+      <c r="C7" s="4" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -975,6 +999,9 @@
       <c r="B8" t="s">
         <v>20</v>
       </c>
+      <c r="C8" s="4" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -983,8 +1010,8 @@
       <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" t="s">
-        <v>12</v>
+      <c r="C9" s="4" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -993,6 +1020,9 @@
       </c>
       <c r="B10" t="s">
         <v>23</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
commit from ahmed 14 June
</commit_message>
<xml_diff>
--- a/code explanation/FIles explanations.xlsx
+++ b/code explanation/FIles explanations.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D8AEE8-C429-4725-A5E2-F4EE50736EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A68BCE-4548-4CBC-B4A8-4B2354DC5D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="126">
   <si>
     <t>MdiADoFunctions</t>
   </si>
@@ -471,10 +471,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -908,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:C10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -937,8 +937,8 @@
       <c r="B2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
+      <c r="C2" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -975,11 +975,11 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -988,7 +988,7 @@
       <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>125</v>
       </c>
     </row>
@@ -999,7 +999,7 @@
       <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1010,7 +1010,7 @@
       <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1021,7 +1021,7 @@
       <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1032,8 +1032,8 @@
       <c r="B11" t="s">
         <v>26</v>
       </c>
-      <c r="C11" t="s">
-        <v>12</v>
+      <c r="C11" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1043,8 +1043,8 @@
       <c r="B12" t="s">
         <v>29</v>
       </c>
-      <c r="C12" t="s">
-        <v>12</v>
+      <c r="C12" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1054,8 +1054,8 @@
       <c r="B13" t="s">
         <v>30</v>
       </c>
-      <c r="C13" t="s">
-        <v>12</v>
+      <c r="C13" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1065,8 +1065,8 @@
       <c r="B14" t="s">
         <v>35</v>
       </c>
-      <c r="C14" t="s">
-        <v>12</v>
+      <c r="C14" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1076,6 +1076,9 @@
       <c r="B15" t="s">
         <v>37</v>
       </c>
+      <c r="C15" s="3" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -1084,8 +1087,8 @@
       <c r="B16" t="s">
         <v>38</v>
       </c>
-      <c r="C16" t="s">
-        <v>12</v>
+      <c r="C16" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -1095,6 +1098,9 @@
       <c r="B17" t="s">
         <v>39</v>
       </c>
+      <c r="C17" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -1103,8 +1109,8 @@
       <c r="B18" t="s">
         <v>35</v>
       </c>
-      <c r="C18" t="s">
-        <v>12</v>
+      <c r="C18" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1149,8 +1155,8 @@
       <c r="B23" t="s">
         <v>35</v>
       </c>
-      <c r="C23" t="s">
-        <v>12</v>
+      <c r="C23" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
commit from ahmed16 june
</commit_message>
<xml_diff>
--- a/code explanation/FIles explanations.xlsx
+++ b/code explanation/FIles explanations.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A68BCE-4548-4CBC-B4A8-4B2354DC5D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DF9763-8BDC-4033-A2B8-13AF47DF68C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -909,7 +909,7 @@
   <dimension ref="A1:C135"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1166,8 +1166,8 @@
       <c r="B24" t="s">
         <v>44</v>
       </c>
-      <c r="C24" t="s">
-        <v>12</v>
+      <c r="C24" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
commit from ahmed 20 june.
</commit_message>
<xml_diff>
--- a/code explanation/FIles explanations.xlsx
+++ b/code explanation/FIles explanations.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DF9763-8BDC-4033-A2B8-13AF47DF68C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0CAF24-51F0-448A-B1FB-C13F4002AE3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="127">
   <si>
     <t>MdiADoFunctions</t>
   </si>
@@ -407,6 +407,9 @@
   </si>
   <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>XMLCalc</t>
   </si>
 </sst>
 </file>
@@ -908,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1177,8 +1180,8 @@
       <c r="B25" t="s">
         <v>35</v>
       </c>
-      <c r="C25" t="s">
-        <v>12</v>
+      <c r="C25" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -1188,30 +1191,30 @@
       <c r="B26" t="s">
         <v>46</v>
       </c>
-      <c r="C26" t="s">
-        <v>12</v>
+      <c r="C26" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" t="s">
-        <v>12</v>
+        <v>126</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" t="s">
-        <v>12</v>
+        <v>47</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1219,40 +1222,40 @@
         <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" t="s">
-        <v>12</v>
+        <v>48</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" t="s">
-        <v>12</v>
+        <v>35</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" t="s">
-        <v>12</v>
+        <v>50</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C32" t="s">
         <v>12</v>
@@ -1260,10 +1263,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
         <v>12</v>
@@ -1271,10 +1274,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="C34" t="s">
         <v>12</v>
@@ -1282,10 +1285,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="C35" t="s">
         <v>12</v>
@@ -1293,7 +1296,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B36" t="s">
         <v>35</v>
@@ -1304,10 +1307,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B37" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="C37" t="s">
         <v>12</v>
@@ -1318,7 +1321,7 @@
         <v>58</v>
       </c>
       <c r="B38" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="C38" t="s">
         <v>12</v>
@@ -1326,10 +1329,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B39" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="C39" t="s">
         <v>12</v>
@@ -1337,10 +1340,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="C40" t="s">
         <v>12</v>
@@ -1348,10 +1351,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C41" t="s">
         <v>12</v>
@@ -1359,10 +1362,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B42" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C42" t="s">
         <v>12</v>
@@ -1370,10 +1373,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C43" t="s">
         <v>12</v>
@@ -1381,10 +1384,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B44" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C44" t="s">
         <v>12</v>
@@ -1392,10 +1395,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="C45" t="s">
         <v>12</v>
@@ -1403,10 +1406,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B46" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="C46" t="s">
         <v>12</v>
@@ -1417,7 +1420,7 @@
         <v>54</v>
       </c>
       <c r="B47" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="C47" t="s">
         <v>12</v>
@@ -1428,9 +1431,20 @@
         <v>54</v>
       </c>
       <c r="B48" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" t="s">
         <v>67</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2156,6 +2170,7 @@
     <mergeCell ref="A6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
commit from ahmed 21 june
</commit_message>
<xml_diff>
--- a/code explanation/FIles explanations.xlsx
+++ b/code explanation/FIles explanations.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0CAF24-51F0-448A-B1FB-C13F4002AE3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44D51D7-97B4-4C5A-9162-1EAF975B0DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -911,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1213,8 +1213,8 @@
       <c r="B28" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>125</v>
+      <c r="C28" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1257,8 +1257,8 @@
       <c r="B32" t="s">
         <v>51</v>
       </c>
-      <c r="C32" t="s">
-        <v>12</v>
+      <c r="C32" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -1268,8 +1268,8 @@
       <c r="B33" t="s">
         <v>53</v>
       </c>
-      <c r="C33" t="s">
-        <v>12</v>
+      <c r="C33" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
commit from ahmed 22 june
</commit_message>
<xml_diff>
--- a/code explanation/FIles explanations.xlsx
+++ b/code explanation/FIles explanations.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44D51D7-97B4-4C5A-9162-1EAF975B0DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD27DD6E-2D9B-41F2-8233-469E1E9D0C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -911,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1279,8 +1279,8 @@
       <c r="B34" t="s">
         <v>35</v>
       </c>
-      <c r="C34" t="s">
-        <v>12</v>
+      <c r="C34" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1290,8 +1290,8 @@
       <c r="B35" t="s">
         <v>56</v>
       </c>
-      <c r="C35" t="s">
-        <v>12</v>
+      <c r="C35" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1301,8 +1301,8 @@
       <c r="B36" t="s">
         <v>35</v>
       </c>
-      <c r="C36" t="s">
-        <v>12</v>
+      <c r="C36" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -1312,8 +1312,8 @@
       <c r="B37" t="s">
         <v>35</v>
       </c>
-      <c r="C37" t="s">
-        <v>12</v>
+      <c r="C37" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
commit from ahmed 27 june
</commit_message>
<xml_diff>
--- a/code explanation/FIles explanations.xlsx
+++ b/code explanation/FIles explanations.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD27DD6E-2D9B-41F2-8233-469E1E9D0C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DE7AEA-3ED0-4CF9-912F-49093B8C50A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="modules" sheetId="1" r:id="rId1"/>
     <sheet name="classes" sheetId="2" r:id="rId2"/>
     <sheet name="code to write" sheetId="3" r:id="rId3"/>
     <sheet name="Libraries" sheetId="4" r:id="rId4"/>
+    <sheet name="Bugs" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="134">
   <si>
     <t>MdiADoFunctions</t>
   </si>
@@ -410,6 +411,27 @@
   </si>
   <si>
     <t>XMLCalc</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>isnumeric()</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Everywhere</t>
+  </si>
+  <si>
+    <t>GetParam()</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
   </si>
 </sst>
 </file>
@@ -911,7 +933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -2202,4 +2224,57 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8BBBBAD-6EAF-4D35-845C-18048AD5969D}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>